<commit_message>
changed the url that caused some issues
</commit_message>
<xml_diff>
--- a/data/city_pics.xlsx
+++ b/data/city_pics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\HE-ARC\annee3\DevWeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\HE-ARC\annee3\DevWeb\Swissdle\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D305A9-121E-4E7C-8A38-58AF5EC5B801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B4D6D5-326A-4A84-84AC-BCEC3355BA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/8/85/City_Zürich_mit_Zürichsee.jpg/1200px-City_Zürich_mit_Zürichsee.jpg</t>
   </si>
@@ -312,9 +312,6 @@
     <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/4/44/Basel_-_M%C3%BCnsterpanorama_Juni_2019.jpg/1280px-Basel_-_M%C3%BCnsterpanorama_Juni_2019.jpg </t>
   </si>
   <si>
-    <t xml:space="preserve">https://media.myswitzerland.com/image/fetch/c_limit,w_1760,h_640/f_auto,q_80,fl_keep_iptc/https://www.myswitzerland.com/-/media/dam/resources/places/r/i/riehen/meta%20page%20image%20all% </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://stadtentwicklung-liestal.ch/wp-content/uploads/2022/09/Bild1-2.jpg </t>
   </si>
   <si>
@@ -330,15 +327,9 @@
     <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/1/1b/Blick_vom_Weinberg_%C3%BCber_Thayngen.jpg </t>
   </si>
   <si>
-    <t xml:space="preserve">https://localcities.rokka.io/web_municipality_image_gallery_v0/b7a324b03e7d28544218adde4104b6c13279a918/2937_neuhausen-am-rheinfall.jpg </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/3/36/Aerial_View_of_Appenzell_14.02.2008_14-45-40.JPG </t>
   </si>
   <si>
-    <t xml:space="preserve">https://gonten.ch/files/Inhalt/Bezirk/Bilder/DSC00393.jpg </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/c/c2/F%C3%BCnfeckpalast_Trogen.jpg </t>
   </si>
   <si>
@@ -423,9 +414,6 @@
     <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/4/4e/Porrentruy_%28JU%29.jpg </t>
   </si>
   <si>
-    <t>https://www.delemont.ch/Htdocs/Images/IF_EntryPage/puid_dd723c23-0f83-44d7-9309-7fa1fee3cf56_eiplace_IF_ImageTextTopPart_3751.png</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/5/51/Moutier_%28JU%29_2.jpg</t>
   </si>
   <si>
@@ -490,6 +478,9 @@
   </si>
   <si>
     <t>Bellinzona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.myswitzerland.com/-/media/dam/resources/places/r/i/riehen/meta%20page%20image%20all% </t>
   </si>
 </sst>
 </file>
@@ -821,17 +812,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="54.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -839,7 +833,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -863,7 +857,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>66</v>
@@ -879,7 +873,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>65</v>
@@ -903,7 +897,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>70</v>
@@ -927,7 +921,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>73</v>
@@ -999,7 +993,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>82</v>
@@ -1023,7 +1017,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>85</v>
@@ -1071,7 +1065,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>91</v>
@@ -1085,7 +1079,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>27</v>
       </c>
@@ -1093,146 +1087,140 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>151</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1240,7 +1228,7 @@
         <v>39</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1248,7 +1236,7 @@
         <v>40</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1256,7 +1244,7 @@
         <v>41</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1264,7 +1252,7 @@
         <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1272,7 +1260,7 @@
         <v>43</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1280,7 +1268,7 @@
         <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1288,7 +1276,7 @@
         <v>45</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1296,7 +1284,7 @@
         <v>46</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1304,15 +1292,15 @@
         <v>47</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1320,7 +1308,7 @@
         <v>48</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1336,7 +1324,7 @@
         <v>51</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1344,109 +1332,106 @@
         <v>52</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
     </row>
   </sheetData>
@@ -1486,50 +1471,47 @@
     <hyperlink ref="B32" r:id="rId33" xr:uid="{9BB1D581-4EED-4933-947A-5F067422187D}"/>
     <hyperlink ref="B33" r:id="rId34" xr:uid="{DF256C8D-14ED-44F8-81CC-AC7A5539ABBC}"/>
     <hyperlink ref="B34" r:id="rId35" xr:uid="{31B785EB-DC9F-4295-BA87-EC219519A221}"/>
-    <hyperlink ref="B35" r:id="rId36" xr:uid="{A53723D5-0A75-45C7-BE6C-38E7BFEA1317}"/>
-    <hyperlink ref="B36" r:id="rId37" xr:uid="{95AC9922-5AB9-45DD-9F17-1528C7F865FF}"/>
-    <hyperlink ref="B37" r:id="rId38" xr:uid="{463DB08F-C586-45FC-9FB8-4953013D6212}"/>
-    <hyperlink ref="B38" r:id="rId39" xr:uid="{2FFA32A7-7AA9-463F-B626-DAB0A330E0F9}"/>
-    <hyperlink ref="B39" r:id="rId40" xr:uid="{295E159A-6434-46DD-A4DE-97F9EA1A7056}"/>
-    <hyperlink ref="B40" r:id="rId41" xr:uid="{9ABD1D4C-B942-40FF-A3E4-0BAC49B8EDA5}"/>
-    <hyperlink ref="B42" r:id="rId42" xr:uid="{553D1F64-5D30-40F6-8BD5-E692C62FDE13}"/>
-    <hyperlink ref="B44" r:id="rId43" xr:uid="{F6CEDEA3-B4F5-44F0-8D72-888A4C351BCA}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{71186C15-06F2-4642-8AA3-FE5E758CD169}"/>
-    <hyperlink ref="B47" r:id="rId45" xr:uid="{DCD8A8B8-4229-4712-8053-A2CCCA9228C0}"/>
-    <hyperlink ref="B49" r:id="rId46" xr:uid="{E441C254-E11D-40C1-B79A-FC5A07A43F0C}"/>
-    <hyperlink ref="B50" r:id="rId47" xr:uid="{EBD1A002-701D-4F9F-8276-D7DE52538EE0}"/>
-    <hyperlink ref="B51" r:id="rId48" xr:uid="{F3654FE4-7653-4745-BCB2-CAEC8723281D}"/>
-    <hyperlink ref="B52" r:id="rId49" xr:uid="{02D9AB1C-0C24-43AA-82D6-FC24DCD45032}"/>
-    <hyperlink ref="B53" r:id="rId50" xr:uid="{CD01456B-5CA2-4112-A5FF-183D7F31EDD2}"/>
-    <hyperlink ref="B54" r:id="rId51" xr:uid="{92DF4642-A45C-4138-9C9E-91A97CEF5375}"/>
-    <hyperlink ref="B55" r:id="rId52" xr:uid="{0E4B2E95-9C7D-4B30-9082-56CDB5DF46BD}"/>
-    <hyperlink ref="B56" r:id="rId53" xr:uid="{631C02BA-9242-42A0-9123-FCCA9CBE50EB}"/>
-    <hyperlink ref="B57" r:id="rId54" xr:uid="{78CB6A6C-0A20-4F6E-8A17-918BD478D362}"/>
-    <hyperlink ref="B58" r:id="rId55" xr:uid="{387C822B-EDB4-4DE8-A370-F05D4452C1C9}"/>
-    <hyperlink ref="B59" r:id="rId56" location="/media/Fichier:Lugano_from_Sighignola.jpg " xr:uid="{F94DB131-4688-4DD1-A1ED-D221A884869A}"/>
-    <hyperlink ref="B60" r:id="rId57" xr:uid="{BE401CE5-3411-4B29-A00C-CCD7EFD1DF42}"/>
-    <hyperlink ref="B61" r:id="rId58" xr:uid="{A7F4285A-8FB0-4105-8DE1-396E52138E2C}"/>
-    <hyperlink ref="B63" r:id="rId59" xr:uid="{C0099A58-6C71-495C-B239-21B92D1684BB}"/>
-    <hyperlink ref="B64" r:id="rId60" xr:uid="{A8262E2D-5281-477E-886E-8F7070B2F9AE}"/>
-    <hyperlink ref="B65" r:id="rId61" xr:uid="{6CE7E38C-E9D1-434A-B344-5D8CF9D2C5C1}"/>
-    <hyperlink ref="B66" r:id="rId62" xr:uid="{3A835213-8AB2-4E42-AB0D-201CD39D0558}"/>
-    <hyperlink ref="B67" r:id="rId63" xr:uid="{0B0A08FD-0950-453D-9C78-3E459AAE152D}"/>
-    <hyperlink ref="B68" r:id="rId64" xr:uid="{107A1E5B-052C-4F82-AB8B-B12A1929EAA4}"/>
-    <hyperlink ref="B69" r:id="rId65" xr:uid="{B2EF5CF7-F836-4375-8498-6BA351CFECCA}"/>
-    <hyperlink ref="B70" r:id="rId66" xr:uid="{93BDD632-7766-4946-B3E1-5B88CA0D98A4}"/>
-    <hyperlink ref="B71" r:id="rId67" xr:uid="{1790F35B-00F5-4C94-AC60-EB78AD54AE50}"/>
-    <hyperlink ref="B72" r:id="rId68" xr:uid="{C5E0C073-53F8-4FF1-A5B1-C875794E4AEA}"/>
-    <hyperlink ref="B73" r:id="rId69" xr:uid="{5D5EF91B-88A1-41A9-BBA2-D44956ADC5D0}"/>
-    <hyperlink ref="B74" r:id="rId70" xr:uid="{1061244E-2EC8-420A-88B2-DFC94C6130C9}"/>
-    <hyperlink ref="B75" r:id="rId71" xr:uid="{A10A8EE6-D84D-4237-B55A-B819C27D13D7}"/>
-    <hyperlink ref="B76" r:id="rId72" xr:uid="{044B6E7E-399B-4D8B-AD3F-F4BB39955076}"/>
-    <hyperlink ref="C75" r:id="rId73" xr:uid="{CF525AE5-F014-4BE7-9108-6F0A6B8E4A3C}"/>
-    <hyperlink ref="B48" r:id="rId74" xr:uid="{46294A07-5C94-4907-9B74-458F067D84A5}"/>
-    <hyperlink ref="B43" r:id="rId75" xr:uid="{6536BF65-118D-4C2E-90FC-8F2FE0042341}"/>
-    <hyperlink ref="C43" r:id="rId76" xr:uid="{05EE60D9-3105-468F-A494-90A66900579D}"/>
-    <hyperlink ref="B46" r:id="rId77" xr:uid="{75B9935F-2C1F-4997-A9A4-BFB51AA0CD21}"/>
-    <hyperlink ref="B41" r:id="rId78" xr:uid="{75E6E455-AF61-4F42-AB23-AC1F3D84CF7F}"/>
-    <hyperlink ref="C41" r:id="rId79" xr:uid="{39AF6C37-0114-4045-A395-6DED1D64879A}"/>
+    <hyperlink ref="B36" r:id="rId36" xr:uid="{95AC9922-5AB9-45DD-9F17-1528C7F865FF}"/>
+    <hyperlink ref="B37" r:id="rId37" xr:uid="{463DB08F-C586-45FC-9FB8-4953013D6212}"/>
+    <hyperlink ref="B38" r:id="rId38" xr:uid="{2FFA32A7-7AA9-463F-B626-DAB0A330E0F9}"/>
+    <hyperlink ref="B39" r:id="rId39" xr:uid="{295E159A-6434-46DD-A4DE-97F9EA1A7056}"/>
+    <hyperlink ref="B40" r:id="rId40" xr:uid="{9ABD1D4C-B942-40FF-A3E4-0BAC49B8EDA5}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{553D1F64-5D30-40F6-8BD5-E692C62FDE13}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{F6CEDEA3-B4F5-44F0-8D72-888A4C351BCA}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{71186C15-06F2-4642-8AA3-FE5E758CD169}"/>
+    <hyperlink ref="B47" r:id="rId44" xr:uid="{DCD8A8B8-4229-4712-8053-A2CCCA9228C0}"/>
+    <hyperlink ref="B49" r:id="rId45" xr:uid="{E441C254-E11D-40C1-B79A-FC5A07A43F0C}"/>
+    <hyperlink ref="B50" r:id="rId46" xr:uid="{EBD1A002-701D-4F9F-8276-D7DE52538EE0}"/>
+    <hyperlink ref="B51" r:id="rId47" xr:uid="{F3654FE4-7653-4745-BCB2-CAEC8723281D}"/>
+    <hyperlink ref="B52" r:id="rId48" xr:uid="{02D9AB1C-0C24-43AA-82D6-FC24DCD45032}"/>
+    <hyperlink ref="B53" r:id="rId49" xr:uid="{CD01456B-5CA2-4112-A5FF-183D7F31EDD2}"/>
+    <hyperlink ref="B54" r:id="rId50" xr:uid="{92DF4642-A45C-4138-9C9E-91A97CEF5375}"/>
+    <hyperlink ref="B55" r:id="rId51" xr:uid="{0E4B2E95-9C7D-4B30-9082-56CDB5DF46BD}"/>
+    <hyperlink ref="B56" r:id="rId52" xr:uid="{631C02BA-9242-42A0-9123-FCCA9CBE50EB}"/>
+    <hyperlink ref="B57" r:id="rId53" xr:uid="{78CB6A6C-0A20-4F6E-8A17-918BD478D362}"/>
+    <hyperlink ref="B58" r:id="rId54" xr:uid="{387C822B-EDB4-4DE8-A370-F05D4452C1C9}"/>
+    <hyperlink ref="B59" r:id="rId55" location="/media/Fichier:Lugano_from_Sighignola.jpg " xr:uid="{F94DB131-4688-4DD1-A1ED-D221A884869A}"/>
+    <hyperlink ref="B60" r:id="rId56" xr:uid="{BE401CE5-3411-4B29-A00C-CCD7EFD1DF42}"/>
+    <hyperlink ref="B61" r:id="rId57" xr:uid="{A7F4285A-8FB0-4105-8DE1-396E52138E2C}"/>
+    <hyperlink ref="B63" r:id="rId58" xr:uid="{C0099A58-6C71-495C-B239-21B92D1684BB}"/>
+    <hyperlink ref="B64" r:id="rId59" xr:uid="{A8262E2D-5281-477E-886E-8F7070B2F9AE}"/>
+    <hyperlink ref="B65" r:id="rId60" xr:uid="{6CE7E38C-E9D1-434A-B344-5D8CF9D2C5C1}"/>
+    <hyperlink ref="B66" r:id="rId61" xr:uid="{3A835213-8AB2-4E42-AB0D-201CD39D0558}"/>
+    <hyperlink ref="B67" r:id="rId62" xr:uid="{0B0A08FD-0950-453D-9C78-3E459AAE152D}"/>
+    <hyperlink ref="B68" r:id="rId63" xr:uid="{107A1E5B-052C-4F82-AB8B-B12A1929EAA4}"/>
+    <hyperlink ref="B69" r:id="rId64" xr:uid="{B2EF5CF7-F836-4375-8498-6BA351CFECCA}"/>
+    <hyperlink ref="B70" r:id="rId65" xr:uid="{93BDD632-7766-4946-B3E1-5B88CA0D98A4}"/>
+    <hyperlink ref="B71" r:id="rId66" xr:uid="{1790F35B-00F5-4C94-AC60-EB78AD54AE50}"/>
+    <hyperlink ref="B72" r:id="rId67" xr:uid="{C5E0C073-53F8-4FF1-A5B1-C875794E4AEA}"/>
+    <hyperlink ref="B73" r:id="rId68" xr:uid="{5D5EF91B-88A1-41A9-BBA2-D44956ADC5D0}"/>
+    <hyperlink ref="B74" r:id="rId69" xr:uid="{1061244E-2EC8-420A-88B2-DFC94C6130C9}"/>
+    <hyperlink ref="B76" r:id="rId70" xr:uid="{044B6E7E-399B-4D8B-AD3F-F4BB39955076}"/>
+    <hyperlink ref="B75" r:id="rId71" xr:uid="{CF525AE5-F014-4BE7-9108-6F0A6B8E4A3C}"/>
+    <hyperlink ref="B48" r:id="rId72" xr:uid="{46294A07-5C94-4907-9B74-458F067D84A5}"/>
+    <hyperlink ref="B43" r:id="rId73" xr:uid="{05EE60D9-3105-468F-A494-90A66900579D}"/>
+    <hyperlink ref="B46" r:id="rId74" xr:uid="{75B9935F-2C1F-4997-A9A4-BFB51AA0CD21}"/>
+    <hyperlink ref="B41" r:id="rId75" xr:uid="{39AF6C37-0114-4045-A395-6DED1D64879A}"/>
+    <hyperlink ref="B35" r:id="rId76" xr:uid="{A53723D5-0A75-45C7-BE6C-38E7BFEA1317}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>